<commit_message>
Template commit before 1st trial
</commit_message>
<xml_diff>
--- a/out/RMRP_2022_AI_consolidated.xlsx
+++ b/out/RMRP_2022_AI_consolidated.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,6 +475,11 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Mexico</t>
@@ -557,6 +562,11 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Mexico</t>
@@ -574,20 +584,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Humanitarian Transportation</t>
+          <t>Food Security</t>
         </is>
       </c>
       <c r="F3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -602,16 +612,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -639,6 +649,11 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Mexico</t>
@@ -656,26 +671,26 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Integration</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -690,10 +705,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -702,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -721,6 +736,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Mexico</t>
@@ -738,20 +758,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Intersector</t>
+          <t>Humanitarian Transportation</t>
         </is>
       </c>
       <c r="F5">
-        <v>308</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>287</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -766,16 +786,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -784,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
@@ -798,11 +818,16 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>CVA Value higher than total</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Mexico</t>
@@ -820,26 +845,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Multipurpose Cash Assistance (MPC)</t>
+          <t>Integration</t>
         </is>
       </c>
       <c r="F6">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="G6">
-        <v>156</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -848,16 +873,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="Q6">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -866,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>156</v>
+        <v>3</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -885,6 +910,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Mexico</t>
@@ -902,65 +932,761 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>Multipurpose Cash Assistance (MPC)</t>
+        </is>
+      </c>
+      <c r="F7">
+        <v>156</v>
+      </c>
+      <c r="G7">
+        <v>156</v>
+      </c>
+      <c r="H7">
+        <v>156</v>
+      </c>
+      <c r="I7">
+        <v>156</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>27</v>
+      </c>
+      <c r="O7">
+        <v>31</v>
+      </c>
+      <c r="P7">
+        <v>49</v>
+      </c>
+      <c r="Q7">
+        <v>49</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>156</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Protection (General)</t>
         </is>
       </c>
-      <c r="F7">
+      <c r="F9">
         <v>42</v>
       </c>
-      <c r="G7">
+      <c r="G9">
         <v>42</v>
       </c>
-      <c r="H7">
+      <c r="H9">
         <v>42</v>
       </c>
-      <c r="I7">
+      <c r="I9">
         <v>42</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>3</v>
       </c>
-      <c r="O7">
+      <c r="O9">
         <v>4</v>
       </c>
-      <c r="P7">
+      <c r="P9">
         <v>16</v>
       </c>
-      <c r="Q7">
+      <c r="Q9">
         <v>19</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
         <v>42</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Protection (GBV)</t>
+        </is>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Protection (Human Trafficking and Smuggling)</t>
+        </is>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Protection (Child Protection)</t>
+        </is>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Shelter</t>
+        </is>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Intersector</t>
+        </is>
+      </c>
+      <c r="F15">
+        <v>308</v>
+      </c>
+      <c r="G15">
+        <v>287</v>
+      </c>
+      <c r="H15">
+        <v>308</v>
+      </c>
+      <c r="I15">
+        <v>301</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>35</v>
+      </c>
+      <c r="O15">
+        <v>41</v>
+      </c>
+      <c r="P15">
+        <v>124</v>
+      </c>
+      <c r="Q15">
+        <v>108</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>287</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>